<commit_message>
function's javascript files with html file
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kihun\Desktop\project_kihun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kihun\Desktop\project_kihun\clone\DevBasicSkills2017-8\kihun_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -72,7 +72,34 @@
     <t>change of plan, for UI design added one more day for partner while waiting partner to be done try to figure out about first function and get advice and help from teacher</t>
   </si>
   <si>
-    <t>Edit little about UI, wait partners answer</t>
+    <t>Edit little about UI, wait partners answer, based on partner's design and work style suggested new plan and still discussion is going on</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>2hr</t>
+  </si>
+  <si>
+    <t>Studied math conception more about it permutation with replacement and without replacement</t>
+  </si>
+  <si>
+    <t>Check about function javascript</t>
+  </si>
+  <si>
+    <t>7hr</t>
+  </si>
+  <si>
+    <t>figure out second function(number system chart) and last function first try out and still figure out first one</t>
+  </si>
+  <si>
+    <t>6hr</t>
+  </si>
+  <si>
+    <t>make other functions basics and try to change first function(number conversion)</t>
+  </si>
+  <si>
+    <t>organize function one html file</t>
   </si>
 </sst>
 </file>
@@ -454,7 +481,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +587,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>30.111000000000001</v>
+        <v>30.11</v>
       </c>
       <c r="B10" s="5">
         <v>0.375</v>
@@ -587,50 +614,102 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="3">
+        <v>2.12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.625</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="3">
+        <v>4.12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="3">
+        <v>5.12</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.625</v>
+      </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="3">
+        <v>6.12</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.75</v>
+      </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>

</xml_diff>

<commit_message>
started Html layout and little edited function with better solution
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>organize function one html file</t>
+  </si>
+  <si>
+    <t>Get advices about function A filtering better solution include method and try to start Html layout</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,12 +715,22 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="3">
+        <v>7.12</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>

</xml_diff>

<commit_message>
check unnecessary files and move away also wrote work_track
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Get advices about function A filtering better solution include method and try to start Html layout</t>
+  </si>
+  <si>
+    <t>After setting up basic layout then try to insert function in every pages until so far function 2 is inserted</t>
   </si>
 </sst>
 </file>
@@ -733,12 +736,22 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="3">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.625</v>
+      </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>

</xml_diff>

<commit_message>
11_12 task implementation for project except truth table
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>After setting up basic layout then try to insert function in every pages until so far function 2 is inserted</t>
+  </si>
+  <si>
+    <t>adding global navigation as famous website's logo and trim little about number chart function</t>
+  </si>
+  <si>
+    <t>finding out error in random values function so try to fix it</t>
   </si>
 </sst>
 </file>
@@ -173,13 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,7 +494,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,20 +761,40 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="3">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.875</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="3">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>

</xml_diff>

<commit_message>
tasks on 12.12 implementation for truth table
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -112,13 +112,25 @@
   </si>
   <si>
     <t>finding out error in random values function so try to fix it</t>
+  </si>
+  <si>
+    <t>kihun han</t>
+  </si>
+  <si>
+    <t>implementation for project html file from function javascript and try to figure out function c ( truth table) more</t>
+  </si>
+  <si>
+    <t>4hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementation for function c (truth table) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +146,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Kunstler Script"/>
+      <family val="4"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,11 +193,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -187,6 +214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +527,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,11 +551,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -797,20 +835,40 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="3">
+        <v>11.12</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="3">
+        <v>12.12</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1037,6 +1095,9 @@
       <c r="F50" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
daily work tracking and made copy of project and progress for random number for sort and different way for showing combinatorics
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t xml:space="preserve">implementation for function c (truth table) </t>
+  </si>
+  <si>
+    <t>4hr 30min</t>
+  </si>
+  <si>
+    <t>puttig html layout more and made combinatorics differently and random value make sort</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,12 +877,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="3">
+        <v>13.12</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>

</xml_diff>

<commit_message>
tasks_14_12 edited page's order and link and little edited last pages
</commit_message>
<xml_diff>
--- a/kihun_project/Work_tracking_.xlsx
+++ b/kihun_project/Work_tracking_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Work tracking sheet</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>puttig html layout more and made combinatorics differently and random value make sort</t>
+  </si>
+  <si>
+    <t>trimed layout more and finish last page's layout and test</t>
   </si>
 </sst>
 </file>
@@ -532,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,12 +898,22 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="3">
+        <v>14.12</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>

</xml_diff>